<commit_message>
Fixes #10 - backup files are in order
</commit_message>
<xml_diff>
--- a/DataMan/Records/static/download-template-Kelly.xlsx
+++ b/DataMan/Records/static/download-template-Kelly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M McCown\SCS\DataMan\Records\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B914A835-7E41-4FD2-BF12-3BA37273F0E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85916E23-2DEF-4DF5-B538-44170CE1375A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="12828" windowHeight="12324" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataMan Upload Details" sheetId="5" r:id="rId1"/>
@@ -1795,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8FB8BE-37D5-48E7-8089-12604CAF4615}">
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -2513,9 +2513,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:J15"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="B21:J21"/>
@@ -2531,6 +2528,9 @@
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2869,8 +2869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="B20" s="56"/>
       <c r="C20" s="57" t="str">
-        <f t="shared" ref="C20:C49" si="0">IF(OR(D20="",$C$2=""), "", $C$2)</f>
+        <f t="shared" ref="C20:C47" si="0">IF(OR(D20="",$C$2=""), "", $C$2)</f>
         <v/>
       </c>
       <c r="D20" s="58"/>
@@ -7999,8 +7999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8051,7 +8051,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="125" t="str">
-        <f>IF(Input!B18="","",$B$2)</f>
+        <f>IF(Input!D18="","",$B$2)</f>
         <v/>
       </c>
       <c r="D2" s="86" t="str">
@@ -8063,7 +8063,7 @@
         <v/>
       </c>
       <c r="F2" s="85" t="str">
-        <f>IF(Input!C18="","",A15)</f>
+        <f>IF(E2="","",$A$15)</f>
         <v/>
       </c>
       <c r="G2" s="87" t="str">
@@ -8087,7 +8087,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="125" t="str">
-        <f>IF(Input!B19="","",$B$3)</f>
+        <f>IF(Input!D19="","",$B$3)</f>
         <v/>
       </c>
       <c r="D3" s="86" t="str">
@@ -8099,7 +8099,7 @@
         <v/>
       </c>
       <c r="F3" s="85" t="str">
-        <f>IF(Input!C19="","",A16)</f>
+        <f>IF(E3="","",$A$15)</f>
         <v/>
       </c>
       <c r="G3" s="87" t="str">
@@ -8122,7 +8122,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="125" t="str">
-        <f>IF(Input!B20="","",$B$4)</f>
+        <f>IF(Input!D20="","",$B$4)</f>
         <v/>
       </c>
       <c r="D4" s="86" t="str">
@@ -8134,7 +8134,7 @@
         <v/>
       </c>
       <c r="F4" s="85" t="str">
-        <f>IF(Input!C20="","",A17)</f>
+        <f t="shared" ref="F4:F31" si="1">IF(E4="","",$A$15)</f>
         <v/>
       </c>
       <c r="G4" s="87" t="str">
@@ -8154,7 +8154,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="125" t="str">
-        <f>IF(Input!B21="","",$B$5)</f>
+        <f>IF(Input!D21="","",$B$5)</f>
         <v/>
       </c>
       <c r="D5" s="86" t="str">
@@ -8166,7 +8166,7 @@
         <v/>
       </c>
       <c r="F5" s="85" t="str">
-        <f>IF(Input!C21="","",A18)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G5" s="87" t="str">
@@ -8189,7 +8189,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="125" t="str">
-        <f>IF(Input!B22="","",$B$6)</f>
+        <f>IF(Input!D22="","",$B$6)</f>
         <v/>
       </c>
       <c r="D6" s="86" t="str">
@@ -8201,7 +8201,7 @@
         <v/>
       </c>
       <c r="F6" s="85" t="str">
-        <f>IF(Input!C22="","",A19)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G6" s="87" t="str">
@@ -8222,7 +8222,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="125" t="str">
-        <f>IF(Input!B23="","",$B$7)</f>
+        <f>IF(Input!D23="","",$B$7)</f>
         <v/>
       </c>
       <c r="D7" s="86" t="str">
@@ -8234,7 +8234,7 @@
         <v/>
       </c>
       <c r="F7" s="85" t="str">
-        <f>IF(Input!C23="","",A20)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G7" s="87" t="str">
@@ -8254,7 +8254,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="125" t="str">
-        <f>IF(Input!B24="","",$B$8)</f>
+        <f>IF(Input!D24="","",$B$8)</f>
         <v/>
       </c>
       <c r="D8" s="86" t="str">
@@ -8266,7 +8266,7 @@
         <v/>
       </c>
       <c r="F8" s="85" t="str">
-        <f>IF(Input!C24="","",A21)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G8" s="87" t="str">
@@ -8286,7 +8286,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="125" t="str">
-        <f>IF(Input!B25="","",$B$9)</f>
+        <f>IF(Input!D25="","",$B$9)</f>
         <v/>
       </c>
       <c r="D9" s="86" t="str">
@@ -8298,7 +8298,7 @@
         <v/>
       </c>
       <c r="F9" s="85" t="str">
-        <f>IF(Input!C25="","",A22)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G9" s="87" t="str">
@@ -8319,7 +8319,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="125" t="str">
-        <f>IF(Input!B26="","",$B$10)</f>
+        <f>IF(Input!D26="","",$B$10)</f>
         <v/>
       </c>
       <c r="D10" s="86" t="str">
@@ -8331,7 +8331,7 @@
         <v/>
       </c>
       <c r="F10" s="85" t="str">
-        <f>IF(Input!C26="","",A23)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G10" s="87" t="str">
@@ -8351,7 +8351,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="125" t="str">
-        <f>IF(Input!B27="","",$B$11)</f>
+        <f>IF(Input!D27="","",$B$11)</f>
         <v/>
       </c>
       <c r="D11" s="86" t="str">
@@ -8363,7 +8363,7 @@
         <v/>
       </c>
       <c r="F11" s="85" t="str">
-        <f>IF(Input!C27="","",A24)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G11" s="87" t="str">
@@ -8383,7 +8383,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="125" t="str">
-        <f>IF(Input!B28="","",$B$12)</f>
+        <f>IF(Input!D28="","",$B$12)</f>
         <v/>
       </c>
       <c r="D12" s="86" t="str">
@@ -8395,7 +8395,7 @@
         <v/>
       </c>
       <c r="F12" s="85" t="str">
-        <f>IF(Input!C28="","",A25)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G12" s="87" t="str">
@@ -8415,7 +8415,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="125" t="str">
-        <f>IF(Input!B29="","",$B$13)</f>
+        <f>IF(Input!D29="","",$B$13)</f>
         <v/>
       </c>
       <c r="D13" s="86" t="str">
@@ -8427,7 +8427,7 @@
         <v/>
       </c>
       <c r="F13" s="85" t="str">
-        <f>IF(Input!C29="","",A26)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G13" s="87" t="str">
@@ -8450,7 +8450,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="125" t="str">
-        <f>IF(Input!B30="","",$B$14)</f>
+        <f>IF(Input!D30="","",$B$14)</f>
         <v/>
       </c>
       <c r="D14" s="86" t="str">
@@ -8462,7 +8462,7 @@
         <v/>
       </c>
       <c r="F14" s="85" t="str">
-        <f>IF(Input!C30="","",A27)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G14" s="87" t="str">
@@ -8485,7 +8485,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="125" t="str">
-        <f>IF(Input!B31="","",$B$15)</f>
+        <f>IF(Input!D31="","",$B$15)</f>
         <v/>
       </c>
       <c r="D15" s="86" t="str">
@@ -8497,7 +8497,7 @@
         <v/>
       </c>
       <c r="F15" s="85" t="str">
-        <f>IF(Input!C31="","",A28)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G15" s="87" t="str">
@@ -8520,7 +8520,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="125" t="str">
-        <f>IF(Input!B32="","",$B$16)</f>
+        <f>IF(Input!D32="","",$B$16)</f>
         <v/>
       </c>
       <c r="D16" s="86" t="str">
@@ -8532,7 +8532,7 @@
         <v/>
       </c>
       <c r="F16" s="85" t="str">
-        <f>IF(Input!C32="","",A29)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G16" s="87" t="str">
@@ -8555,7 +8555,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="125" t="str">
-        <f>IF(Input!B33="","",$B$17)</f>
+        <f>IF(Input!D33="","",$B$17)</f>
         <v/>
       </c>
       <c r="D17" s="86" t="str">
@@ -8567,7 +8567,7 @@
         <v/>
       </c>
       <c r="F17" s="85" t="str">
-        <f>IF(Input!C33="","",A30)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G17" s="87" t="str">
@@ -8587,7 +8587,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="125" t="str">
-        <f>IF(Input!B34="","",$B$18)</f>
+        <f>IF(Input!D34="","",$B$18)</f>
         <v/>
       </c>
       <c r="D18" s="86" t="str">
@@ -8599,7 +8599,7 @@
         <v/>
       </c>
       <c r="F18" s="85" t="str">
-        <f>IF(Input!C34="","",A31)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G18" s="87" t="str">
@@ -8619,7 +8619,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="125" t="str">
-        <f>IF(Input!B35="","",$B$19)</f>
+        <f>IF(Input!D35="","",$B$19)</f>
         <v/>
       </c>
       <c r="D19" s="86" t="str">
@@ -8631,7 +8631,7 @@
         <v/>
       </c>
       <c r="F19" s="85" t="str">
-        <f>IF(Input!C35="","",A32)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G19" s="87" t="str">
@@ -8651,7 +8651,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="125" t="str">
-        <f>IF(Input!B36="","",$B$20)</f>
+        <f>IF(Input!D36="","",$B$20)</f>
         <v/>
       </c>
       <c r="D20" s="86" t="str">
@@ -8663,7 +8663,7 @@
         <v/>
       </c>
       <c r="F20" s="85" t="str">
-        <f>IF(Input!C36="","",A33)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G20" s="87" t="str">
@@ -8686,7 +8686,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="125" t="str">
-        <f>IF(Input!B37="","",$B$21)</f>
+        <f>IF(Input!D37="","",$B$21)</f>
         <v/>
       </c>
       <c r="D21" s="86" t="str">
@@ -8698,7 +8698,7 @@
         <v/>
       </c>
       <c r="F21" s="85" t="str">
-        <f>IF(Input!C37="","",A34)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G21" s="87" t="str">
@@ -8721,7 +8721,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="125" t="str">
-        <f>IF(Input!B38="","",$B$22)</f>
+        <f>IF(Input!D38="","",$B$22)</f>
         <v/>
       </c>
       <c r="D22" s="86" t="str">
@@ -8733,7 +8733,7 @@
         <v/>
       </c>
       <c r="F22" s="85" t="str">
-        <f>IF(Input!C38="","",A35)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G22" s="87" t="str">
@@ -8756,7 +8756,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="125" t="str">
-        <f>IF(Input!B39="","",$B$23)</f>
+        <f>IF(Input!D39="","",$B$23)</f>
         <v/>
       </c>
       <c r="D23" s="86" t="str">
@@ -8768,7 +8768,7 @@
         <v/>
       </c>
       <c r="F23" s="85" t="str">
-        <f>IF(Input!C39="","",A36)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G23" s="87" t="str">
@@ -8791,7 +8791,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="125" t="str">
-        <f>IF(Input!B40="","",$B$24)</f>
+        <f>IF(Input!D40="","",$B$24)</f>
         <v/>
       </c>
       <c r="D24" s="86" t="str">
@@ -8803,7 +8803,7 @@
         <v/>
       </c>
       <c r="F24" s="85" t="str">
-        <f>IF(Input!C40="","",A37)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G24" s="87" t="str">
@@ -8823,7 +8823,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="125" t="str">
-        <f>IF(Input!B41="","",$B$25)</f>
+        <f>IF(Input!D41="","",$B$25)</f>
         <v/>
       </c>
       <c r="D25" s="86" t="str">
@@ -8835,7 +8835,7 @@
         <v/>
       </c>
       <c r="F25" s="85" t="str">
-        <f>IF(Input!C41="","",A38)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G25" s="87" t="str">
@@ -8855,7 +8855,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="125" t="str">
-        <f>IF(Input!B42="","",$B$26)</f>
+        <f>IF(Input!D42="","",$B$26)</f>
         <v/>
       </c>
       <c r="D26" s="86" t="str">
@@ -8867,7 +8867,7 @@
         <v/>
       </c>
       <c r="F26" s="85" t="str">
-        <f>IF(Input!C42="","",A39)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G26" s="87" t="str">
@@ -8887,7 +8887,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="125" t="str">
-        <f>IF(Input!B43="","",$B$27)</f>
+        <f>IF(Input!D43="","",$B$27)</f>
         <v/>
       </c>
       <c r="D27" s="86" t="str">
@@ -8899,7 +8899,7 @@
         <v/>
       </c>
       <c r="F27" s="85" t="str">
-        <f>IF(Input!C43="","",A40)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G27" s="87" t="str">
@@ -8919,7 +8919,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="125" t="str">
-        <f>IF(Input!B44="","",$B$28)</f>
+        <f>IF(Input!D44="","",$B$28)</f>
         <v/>
       </c>
       <c r="D28" s="86" t="str">
@@ -8931,7 +8931,7 @@
         <v/>
       </c>
       <c r="F28" s="85" t="str">
-        <f>IF(Input!C44="","",A41)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G28" s="87" t="str">
@@ -8952,7 +8952,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="125" t="str">
-        <f>IF(Input!B45="","",$B$29)</f>
+        <f>IF(Input!D45="","",$B$29)</f>
         <v/>
       </c>
       <c r="D29" s="86" t="str">
@@ -8964,7 +8964,7 @@
         <v/>
       </c>
       <c r="F29" s="85" t="str">
-        <f>IF(Input!C45="","",A42)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G29" s="87" t="str">
@@ -8984,7 +8984,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="125" t="str">
-        <f>IF(Input!B46="","",$B$30)</f>
+        <f>IF(Input!D46="","",$B$30)</f>
         <v/>
       </c>
       <c r="D30" s="86" t="str">
@@ -8996,7 +8996,7 @@
         <v/>
       </c>
       <c r="F30" s="85" t="str">
-        <f>IF(Input!C46="","",A43)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G30" s="87" t="str">
@@ -9016,7 +9016,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="128" t="str">
-        <f>IF(Input!B47="","",$B$31)</f>
+        <f>IF(Input!D47="","",$B$31)</f>
         <v/>
       </c>
       <c r="D31" s="86" t="str">
@@ -9028,7 +9028,7 @@
         <v/>
       </c>
       <c r="F31" s="85" t="str">
-        <f>IF(Input!C47="","",A44)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G31" s="87" t="str">
@@ -9046,7 +9046,7 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C32" s="84"/>
       <c r="D32" s="83" t="str">
-        <f t="shared" ref="D32:D38" si="1">IF(E32="","","Experimental")</f>
+        <f t="shared" ref="D32:D38" si="2">IF(E32="","","Experimental")</f>
         <v/>
       </c>
       <c r="E32" s="84"/>
@@ -9059,7 +9059,7 @@
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D33" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E33" s="84"/>
@@ -9075,7 +9075,7 @@
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D34" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E34" s="84"/>
@@ -9091,7 +9091,7 @@
     </row>
     <row r="35" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D35" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E35" s="84"/>
@@ -9107,7 +9107,7 @@
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D36" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E36" s="84"/>
@@ -9123,7 +9123,7 @@
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D37" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E37" s="84"/>
@@ -9138,7 +9138,7 @@
     </row>
     <row r="38" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D38" s="83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="E38" s="84"/>
@@ -9153,7 +9153,7 @@
     </row>
     <row r="39" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D39" s="83" t="str">
-        <f t="shared" ref="D39:D60" si="2">IF(E37="","","Experimental")</f>
+        <f t="shared" ref="D39:D60" si="3">IF(E37="","","Experimental")</f>
         <v/>
       </c>
       <c r="E39" s="84"/>
@@ -9168,7 +9168,7 @@
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D40" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E40" s="84"/>
@@ -9183,7 +9183,7 @@
     </row>
     <row r="41" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D41" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E41" s="84"/>
@@ -9198,7 +9198,7 @@
     </row>
     <row r="42" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D42" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E42" s="84"/>
@@ -9213,7 +9213,7 @@
     </row>
     <row r="43" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D43" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E43" s="84"/>
@@ -9228,7 +9228,7 @@
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D44" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E44" s="84"/>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="45" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D45" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E45" s="84"/>
@@ -9258,7 +9258,7 @@
     </row>
     <row r="46" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D46" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E46" s="84"/>
@@ -9273,7 +9273,7 @@
     </row>
     <row r="47" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D47" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E47" s="84"/>
@@ -9288,7 +9288,7 @@
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D48" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E48" s="84"/>
@@ -9303,7 +9303,7 @@
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D49" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E49" s="84"/>
@@ -9318,7 +9318,7 @@
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D50" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E50" s="84"/>
@@ -9333,7 +9333,7 @@
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D51" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E51" s="84"/>
@@ -9348,7 +9348,7 @@
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D52" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E52" s="84"/>
@@ -9363,7 +9363,7 @@
     </row>
     <row r="53" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D53" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E53" s="84"/>
@@ -9378,7 +9378,7 @@
     </row>
     <row r="54" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D54" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E54" s="84"/>
@@ -9393,7 +9393,7 @@
     </row>
     <row r="55" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D55" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E55" s="84"/>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D56" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E56" s="84"/>
@@ -9423,7 +9423,7 @@
     </row>
     <row r="57" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D57" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E57" s="84"/>
@@ -9438,7 +9438,7 @@
     </row>
     <row r="58" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D58" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E58" s="84"/>
@@ -9453,7 +9453,7 @@
     </row>
     <row r="59" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D59" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E59" s="84"/>
@@ -9468,7 +9468,7 @@
     </row>
     <row r="60" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D60" s="83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="E60" s="84"/>

</xml_diff>

<commit_message>
Added helpful error messages to upload; fixed #15
</commit_message>
<xml_diff>
--- a/DataMan/Records/static/download-template-Kelly.xlsx
+++ b/DataMan/Records/static/download-template-Kelly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M McCown\SCS\DataMan\Records\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85916E23-2DEF-4DF5-B538-44170CE1375A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F56E3F-BEBB-428B-A3BA-CFC9A01610F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataMan Upload Details" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="150">
   <si>
     <t>Species</t>
   </si>
@@ -394,9 +394,6 @@
     <t>C:/User/Example/data/</t>
   </si>
   <si>
-    <t>Tissue Source Identifier</t>
-  </si>
-  <si>
     <t>Hela</t>
   </si>
   <si>
@@ -502,7 +499,7 @@
     <t>Ryan Kellly</t>
   </si>
   <si>
-    <t>EXP</t>
+    <t>Individual (Tissue Source) Identifier</t>
   </si>
 </sst>
 </file>
@@ -2513,7 +2510,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="A14:J14"/>
@@ -2531,6 +2527,7 @@
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="A16:J16"/>
     <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="9" spans="1:13" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2870,7 +2867,7 @@
   <dimension ref="A1:T1007"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2881,7 +2878,7 @@
     <col min="7" max="7" width="10.109375" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" customWidth="1"/>
     <col min="11" max="11" width="23.109375" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" customWidth="1"/>
     <col min="13" max="13" width="18.109375" customWidth="1"/>
@@ -2914,9 +2911,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="148"/>
-      <c r="C2" s="149" t="s">
-        <v>150</v>
-      </c>
+      <c r="C2" s="149"/>
       <c r="D2" s="149"/>
       <c r="E2" s="149"/>
       <c r="F2" s="149"/>
@@ -2933,7 +2928,7 @@
       </c>
       <c r="B3" s="152"/>
       <c r="C3" s="150" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="150"/>
       <c r="E3" s="150"/>
@@ -3042,7 +3037,7 @@
       <c r="I11" s="77"/>
       <c r="J11" s="44"/>
       <c r="N11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -3082,7 +3077,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>6</v>
@@ -3097,7 +3092,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>27</v>
@@ -3109,22 +3104,22 @@
         <v>28</v>
       </c>
       <c r="N15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q15" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q15" s="69" t="s">
-        <v>117</v>
-      </c>
       <c r="R15" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="T15" s="69"/>
     </row>
@@ -3139,22 +3134,22 @@
         <v>100</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16" s="34" t="s">
         <v>33</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K16" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L16" s="90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M16" s="91" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N16" s="12" t="str">
         <f>Other!A2</f>
@@ -3169,10 +3164,10 @@
         <v>HoneyWell - HPLC grade Water - Lot 123456789</v>
       </c>
       <c r="Q16" s="70" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R16" s="76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S16" s="76">
         <v>28436</v>
@@ -8000,7 +7995,7 @@
   <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8073,7 +8068,7 @@
       <c r="H2" s="45"/>
       <c r="J2" s="44"/>
       <c r="K2" s="88" t="str">
-        <f>IF(Input!C18="","",A17)</f>
+        <f>IF(Input!C18="","",$A$17)</f>
         <v/>
       </c>
       <c r="L2" s="126"/>
@@ -8109,7 +8104,7 @@
       <c r="H3" s="45"/>
       <c r="J3" s="44"/>
       <c r="K3" s="88" t="str">
-        <f>IF(Input!C19="","",A18)</f>
+        <f>IF(Input!C19="","",$A$17)</f>
         <v/>
       </c>
       <c r="L3" s="126"/>
@@ -8144,7 +8139,7 @@
       <c r="H4" s="45"/>
       <c r="J4" s="44"/>
       <c r="K4" s="88" t="str">
-        <f>IF(Input!C20="","",A19)</f>
+        <f>IF(Input!C20="","",$A$17)</f>
         <v/>
       </c>
       <c r="L4" s="126"/>
@@ -8176,7 +8171,7 @@
       <c r="H5" s="45"/>
       <c r="J5" s="44"/>
       <c r="K5" s="88" t="str">
-        <f>IF(Input!C21="","",A20)</f>
+        <f>IF(Input!C21="","",$A$17)</f>
         <v/>
       </c>
       <c r="L5" s="126"/>
@@ -8211,7 +8206,7 @@
       <c r="H6" s="45"/>
       <c r="J6" s="44"/>
       <c r="K6" s="88" t="str">
-        <f>IF(Input!C22="","",A21)</f>
+        <f>IF(Input!C22="","",$A$17)</f>
         <v/>
       </c>
       <c r="L6" s="126"/>
@@ -8244,7 +8239,7 @@
       <c r="H7" s="45"/>
       <c r="J7" s="44"/>
       <c r="K7" s="88" t="str">
-        <f>IF(Input!C23="","",A22)</f>
+        <f>IF(Input!C23="","",$A$17)</f>
         <v/>
       </c>
       <c r="L7" s="126"/>
@@ -8276,7 +8271,7 @@
       <c r="H8" s="45"/>
       <c r="J8" s="44"/>
       <c r="K8" s="88" t="str">
-        <f>IF(Input!C24="","",A23)</f>
+        <f>IF(Input!C24="","",$A$17)</f>
         <v/>
       </c>
       <c r="L8" s="126"/>
@@ -8308,7 +8303,7 @@
       <c r="H9" s="45"/>
       <c r="J9" s="44"/>
       <c r="K9" s="88" t="str">
-        <f>IF(Input!C25="","",A24)</f>
+        <f>IF(Input!C25="","",$A$17)</f>
         <v/>
       </c>
       <c r="L9" s="126"/>
@@ -8341,7 +8336,7 @@
       <c r="H10" s="45"/>
       <c r="J10" s="44"/>
       <c r="K10" s="88" t="str">
-        <f>IF(Input!C26="","",A25)</f>
+        <f>IF(Input!C26="","",$A$17)</f>
         <v/>
       </c>
       <c r="L10" s="126"/>
@@ -8373,7 +8368,7 @@
       <c r="H11" s="45"/>
       <c r="J11" s="44"/>
       <c r="K11" s="88" t="str">
-        <f>IF(Input!C27="","",A26)</f>
+        <f>IF(Input!C27="","",$A$17)</f>
         <v/>
       </c>
       <c r="L11" s="126"/>
@@ -8405,7 +8400,7 @@
       <c r="H12" s="45"/>
       <c r="J12" s="44"/>
       <c r="K12" s="88" t="str">
-        <f>IF(Input!C28="","",A27)</f>
+        <f>IF(Input!C28="","",$A$17)</f>
         <v/>
       </c>
       <c r="L12" s="126"/>
@@ -8437,7 +8432,7 @@
       <c r="H13" s="45"/>
       <c r="J13" s="44"/>
       <c r="K13" s="88" t="str">
-        <f>IF(Input!C29="","",A28)</f>
+        <f>IF(Input!C29="","",$A$17)</f>
         <v/>
       </c>
       <c r="L13" s="126"/>
@@ -8472,7 +8467,7 @@
       <c r="H14" s="45"/>
       <c r="J14" s="44"/>
       <c r="K14" s="88" t="str">
-        <f>IF(Input!C30="","",A29)</f>
+        <f>IF(Input!C30="","",$A$17)</f>
         <v/>
       </c>
       <c r="L14" s="126"/>
@@ -8507,7 +8502,7 @@
       <c r="H15" s="45"/>
       <c r="J15" s="44"/>
       <c r="K15" s="88" t="str">
-        <f>IF(Input!C31="","",A30)</f>
+        <f>IF(Input!C31="","",$A$17)</f>
         <v/>
       </c>
       <c r="L15" s="126"/>
@@ -8542,7 +8537,7 @@
       <c r="H16" s="45"/>
       <c r="J16" s="44"/>
       <c r="K16" s="88" t="str">
-        <f>IF(Input!C32="","",A31)</f>
+        <f>IF(Input!C32="","",$A$17)</f>
         <v/>
       </c>
       <c r="L16" s="126"/>
@@ -8577,7 +8572,7 @@
       <c r="H17" s="45"/>
       <c r="J17" s="44"/>
       <c r="K17" s="88" t="str">
-        <f>IF(Input!C33="","",A32)</f>
+        <f>IF(Input!C33="","",$A$17)</f>
         <v/>
       </c>
       <c r="L17" s="126"/>
@@ -8609,7 +8604,7 @@
       <c r="H18" s="45"/>
       <c r="J18" s="44"/>
       <c r="K18" s="88" t="str">
-        <f>IF(Input!C34="","",A33)</f>
+        <f>IF(Input!C34="","",$A$17)</f>
         <v/>
       </c>
       <c r="L18" s="126"/>
@@ -8641,7 +8636,7 @@
       <c r="H19" s="45"/>
       <c r="J19" s="44"/>
       <c r="K19" s="88" t="str">
-        <f>IF(Input!C35="","",A34)</f>
+        <f>IF(Input!C35="","",$A$17)</f>
         <v/>
       </c>
       <c r="L19" s="126"/>
@@ -8673,14 +8668,14 @@
       <c r="H20" s="45"/>
       <c r="J20" s="44"/>
       <c r="K20" s="88" t="str">
-        <f>IF(Input!C36="","",A35)</f>
+        <f>IF(Input!C36="","",$A$17)</f>
         <v/>
       </c>
       <c r="L20" s="126"/>
     </row>
     <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -8708,14 +8703,14 @@
       <c r="H21" s="45"/>
       <c r="J21" s="44"/>
       <c r="K21" s="88" t="str">
-        <f>IF(Input!C37="","",A36)</f>
+        <f>IF(Input!C37="","",$A$17)</f>
         <v/>
       </c>
       <c r="L21" s="126"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -8743,14 +8738,14 @@
       <c r="H22" s="45"/>
       <c r="J22" s="44"/>
       <c r="K22" s="88" t="str">
-        <f>IF(Input!C38="","",A37)</f>
+        <f>IF(Input!C38="","",$A$17)</f>
         <v/>
       </c>
       <c r="L22" s="126"/>
     </row>
     <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -8778,14 +8773,14 @@
       <c r="H23" s="45"/>
       <c r="J23" s="44"/>
       <c r="K23" s="88" t="str">
-        <f>IF(Input!C39="","",A38)</f>
+        <f>IF(Input!C39="","",$A$17)</f>
         <v/>
       </c>
       <c r="L23" s="126"/>
     </row>
     <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -8813,7 +8808,7 @@
       <c r="H24" s="45"/>
       <c r="J24" s="44"/>
       <c r="K24" s="88" t="str">
-        <f>IF(Input!C40="","",A39)</f>
+        <f>IF(Input!C40="","",$A$17)</f>
         <v/>
       </c>
       <c r="L24" s="126"/>
@@ -8845,7 +8840,7 @@
       <c r="H25" s="45"/>
       <c r="J25" s="44"/>
       <c r="K25" s="88" t="str">
-        <f>IF(Input!C41="","",A40)</f>
+        <f>IF(Input!C41="","",$A$17)</f>
         <v/>
       </c>
       <c r="L25" s="126"/>
@@ -8877,7 +8872,7 @@
       <c r="H26" s="45"/>
       <c r="J26" s="44"/>
       <c r="K26" s="88" t="str">
-        <f>IF(Input!C42="","",A41)</f>
+        <f>IF(Input!C42="","",$A$17)</f>
         <v/>
       </c>
       <c r="L26" s="126"/>
@@ -8909,7 +8904,7 @@
       <c r="H27" s="45"/>
       <c r="J27" s="44"/>
       <c r="K27" s="88" t="str">
-        <f>IF(Input!C43="","",A42)</f>
+        <f>IF(Input!C43="","",$A$17)</f>
         <v/>
       </c>
       <c r="L27" s="126"/>
@@ -8941,7 +8936,7 @@
       <c r="H28" s="45"/>
       <c r="J28" s="44"/>
       <c r="K28" s="88" t="str">
-        <f>IF(Input!C44="","",A43)</f>
+        <f>IF(Input!C44="","",$A$17)</f>
         <v/>
       </c>
       <c r="L28" s="126"/>
@@ -8974,7 +8969,7 @@
       <c r="H29" s="45"/>
       <c r="J29" s="44"/>
       <c r="K29" s="88" t="str">
-        <f>IF(Input!C45="","",A44)</f>
+        <f>IF(Input!C45="","",$A$17)</f>
         <v/>
       </c>
       <c r="L29" s="126"/>
@@ -9006,7 +9001,7 @@
       <c r="H30" s="45"/>
       <c r="J30" s="44"/>
       <c r="K30" s="88" t="str">
-        <f>IF(Input!C46="","",A45)</f>
+        <f>IF(Input!C46="","",$A$17)</f>
         <v/>
       </c>
       <c r="L30" s="126"/>
@@ -9038,12 +9033,12 @@
       <c r="H31" s="45"/>
       <c r="J31" s="44"/>
       <c r="K31" s="88" t="str">
-        <f>IF(Input!C47="","",A46)</f>
+        <f>IF(Input!C47="","",$A$17)</f>
         <v/>
       </c>
       <c r="L31" s="126"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="84"/>
       <c r="D32" s="83" t="str">
         <f t="shared" ref="D32:D38" si="2">IF(E32="","","Experimental")</f>
@@ -9054,10 +9049,13 @@
       <c r="G32" s="83"/>
       <c r="H32" s="44"/>
       <c r="J32" s="44"/>
-      <c r="K32" s="84"/>
+      <c r="K32" s="88" t="str">
+        <f>IF(Input!C48="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L32" s="83"/>
     </row>
-    <row r="33" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D33" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9067,13 +9065,16 @@
       <c r="G33" s="83"/>
       <c r="H33" s="44"/>
       <c r="J33" s="44"/>
-      <c r="K33" s="84"/>
+      <c r="K33" s="88" t="str">
+        <f>IF(Input!C49="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L33" s="83"/>
       <c r="M33" s="44"/>
       <c r="N33" s="45"/>
       <c r="O33" s="45"/>
     </row>
-    <row r="34" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D34" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9083,13 +9084,16 @@
       <c r="G34" s="83"/>
       <c r="H34" s="44"/>
       <c r="J34" s="44"/>
-      <c r="K34" s="84"/>
+      <c r="K34" s="88" t="str">
+        <f>IF(Input!C50="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L34" s="83"/>
       <c r="M34" s="44"/>
       <c r="N34" s="45"/>
       <c r="O34" s="45"/>
     </row>
-    <row r="35" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9099,13 +9103,16 @@
       <c r="G35" s="83"/>
       <c r="H35" s="44"/>
       <c r="J35" s="44"/>
-      <c r="K35" s="84"/>
+      <c r="K35" s="88" t="str">
+        <f>IF(Input!C51="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L35" s="83"/>
       <c r="M35" s="44"/>
       <c r="N35" s="45"/>
       <c r="O35" s="45"/>
     </row>
-    <row r="36" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D36" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9115,13 +9122,16 @@
       <c r="G36" s="83"/>
       <c r="H36" s="44"/>
       <c r="J36" s="44"/>
-      <c r="K36" s="84"/>
+      <c r="K36" s="88" t="str">
+        <f>IF(Input!C52="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L36" s="83"/>
       <c r="M36" s="44"/>
       <c r="N36" s="45"/>
       <c r="O36" s="45"/>
     </row>
-    <row r="37" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D37" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9131,12 +9141,15 @@
       <c r="G37" s="83"/>
       <c r="H37" s="44"/>
       <c r="J37" s="44"/>
-      <c r="K37" s="84"/>
+      <c r="K37" s="88" t="str">
+        <f>IF(Input!C53="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L37" s="83"/>
       <c r="N37" s="45"/>
       <c r="O37" s="45"/>
     </row>
-    <row r="38" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D38" s="83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9146,12 +9159,15 @@
       <c r="G38" s="83"/>
       <c r="H38" s="44"/>
       <c r="J38" s="44"/>
-      <c r="K38" s="84"/>
+      <c r="K38" s="88" t="str">
+        <f>IF(Input!C54="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L38" s="83"/>
       <c r="N38" s="45"/>
       <c r="O38" s="45"/>
     </row>
-    <row r="39" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="83" t="str">
         <f t="shared" ref="D39:D60" si="3">IF(E37="","","Experimental")</f>
         <v/>
@@ -9161,12 +9177,15 @@
       <c r="G39" s="83"/>
       <c r="H39" s="44"/>
       <c r="J39" s="44"/>
-      <c r="K39" s="84"/>
+      <c r="K39" s="88" t="str">
+        <f>IF(Input!C55="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L39" s="83"/>
       <c r="N39" s="45"/>
       <c r="O39" s="45"/>
     </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D40" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9176,12 +9195,15 @@
       <c r="G40" s="83"/>
       <c r="H40" s="44"/>
       <c r="J40" s="44"/>
-      <c r="K40" s="84"/>
+      <c r="K40" s="88" t="str">
+        <f>IF(Input!C56="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L40" s="83"/>
       <c r="N40" s="45"/>
       <c r="O40" s="45"/>
     </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D41" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9191,12 +9213,15 @@
       <c r="G41" s="83"/>
       <c r="H41" s="44"/>
       <c r="J41" s="44"/>
-      <c r="K41" s="84"/>
+      <c r="K41" s="88" t="str">
+        <f>IF(Input!C57="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L41" s="83"/>
       <c r="N41" s="45"/>
       <c r="O41" s="45"/>
     </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D42" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9206,12 +9231,15 @@
       <c r="G42" s="83"/>
       <c r="H42" s="44"/>
       <c r="J42" s="44"/>
-      <c r="K42" s="84"/>
+      <c r="K42" s="88" t="str">
+        <f>IF(Input!C58="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L42" s="83"/>
       <c r="N42" s="45"/>
       <c r="O42" s="45"/>
     </row>
-    <row r="43" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D43" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9221,12 +9249,15 @@
       <c r="G43" s="83"/>
       <c r="H43" s="44"/>
       <c r="J43" s="44"/>
-      <c r="K43" s="84"/>
+      <c r="K43" s="88" t="str">
+        <f>IF(Input!C59="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L43" s="83"/>
       <c r="N43" s="45"/>
       <c r="O43" s="45"/>
     </row>
-    <row r="44" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D44" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9236,12 +9267,15 @@
       <c r="G44" s="83"/>
       <c r="H44" s="44"/>
       <c r="J44" s="44"/>
-      <c r="K44" s="84"/>
+      <c r="K44" s="88" t="str">
+        <f>IF(Input!C60="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L44" s="83"/>
       <c r="N44" s="45"/>
       <c r="O44" s="45"/>
     </row>
-    <row r="45" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D45" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9251,12 +9285,15 @@
       <c r="G45" s="83"/>
       <c r="H45" s="44"/>
       <c r="J45" s="44"/>
-      <c r="K45" s="84"/>
+      <c r="K45" s="88" t="str">
+        <f>IF(Input!C61="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L45" s="83"/>
       <c r="N45" s="45"/>
       <c r="O45" s="45"/>
     </row>
-    <row r="46" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D46" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9266,12 +9303,15 @@
       <c r="G46" s="83"/>
       <c r="H46" s="44"/>
       <c r="J46" s="44"/>
-      <c r="K46" s="84"/>
+      <c r="K46" s="88" t="str">
+        <f>IF(Input!C62="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L46" s="83"/>
       <c r="N46" s="45"/>
       <c r="O46" s="45"/>
     </row>
-    <row r="47" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D47" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9281,12 +9321,15 @@
       <c r="G47" s="83"/>
       <c r="H47" s="44"/>
       <c r="J47" s="44"/>
-      <c r="K47" s="84"/>
+      <c r="K47" s="88" t="str">
+        <f>IF(Input!C63="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L47" s="83"/>
       <c r="N47" s="45"/>
       <c r="O47" s="45"/>
     </row>
-    <row r="48" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D48" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9296,12 +9339,15 @@
       <c r="G48" s="83"/>
       <c r="H48" s="44"/>
       <c r="J48" s="44"/>
-      <c r="K48" s="84"/>
+      <c r="K48" s="88" t="str">
+        <f>IF(Input!C64="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L48" s="83"/>
       <c r="N48" s="45"/>
       <c r="O48" s="45"/>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D49" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9311,12 +9357,15 @@
       <c r="G49" s="83"/>
       <c r="H49" s="44"/>
       <c r="J49" s="44"/>
-      <c r="K49" s="84"/>
+      <c r="K49" s="88" t="str">
+        <f>IF(Input!C65="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L49" s="83"/>
       <c r="N49" s="45"/>
       <c r="O49" s="45"/>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D50" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9326,12 +9375,15 @@
       <c r="G50" s="83"/>
       <c r="H50" s="44"/>
       <c r="J50" s="44"/>
-      <c r="K50" s="84"/>
+      <c r="K50" s="88" t="str">
+        <f>IF(Input!C66="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L50" s="83"/>
       <c r="N50" s="45"/>
       <c r="O50" s="45"/>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D51" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9341,12 +9393,15 @@
       <c r="G51" s="83"/>
       <c r="H51" s="44"/>
       <c r="J51" s="44"/>
-      <c r="K51" s="84"/>
+      <c r="K51" s="88" t="str">
+        <f>IF(Input!C67="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L51" s="83"/>
       <c r="N51" s="45"/>
       <c r="O51" s="45"/>
     </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D52" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9356,12 +9411,15 @@
       <c r="G52" s="83"/>
       <c r="H52" s="44"/>
       <c r="J52" s="44"/>
-      <c r="K52" s="84"/>
+      <c r="K52" s="88" t="str">
+        <f>IF(Input!C68="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L52" s="83"/>
       <c r="N52" s="45"/>
       <c r="O52" s="45"/>
     </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9371,12 +9429,15 @@
       <c r="G53" s="83"/>
       <c r="H53" s="44"/>
       <c r="J53" s="44"/>
-      <c r="K53" s="84"/>
+      <c r="K53" s="88" t="str">
+        <f>IF(Input!C69="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L53" s="83"/>
       <c r="N53" s="45"/>
       <c r="O53" s="45"/>
     </row>
-    <row r="54" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D54" s="83" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -9386,7 +9447,10 @@
       <c r="G54" s="83"/>
       <c r="H54" s="44"/>
       <c r="J54" s="44"/>
-      <c r="K54" s="84"/>
+      <c r="K54" s="88" t="str">
+        <f>IF(Input!C70="","",$A$17)</f>
+        <v/>
+      </c>
       <c r="L54" s="83"/>
       <c r="N54" s="45"/>
       <c r="O54" s="45"/>
@@ -9584,34 +9648,34 @@
         <v>2</v>
       </c>
       <c r="B1" s="111" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="111" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="D1" s="111" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="111" t="s">
+      <c r="E1" s="127" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="127" t="s">
-        <v>143</v>
-      </c>
       <c r="F1" s="112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="116" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="104" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="45">
         <v>1</v>
@@ -9995,16 +10059,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="E1" s="77"/>
     </row>
@@ -10014,10 +10078,10 @@
         <v>HoneyWell - HPLC grade Water - Lot 123456789</v>
       </c>
       <c r="B2" s="96" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="97" t="s">
         <v>136</v>
-      </c>
-      <c r="C2" s="97" t="s">
-        <v>137</v>
       </c>
       <c r="D2" s="98">
         <v>123456789</v>
@@ -10037,10 +10101,10 @@
         <v>HoneyWell - HPLC grade Water - Lot 123456789</v>
       </c>
       <c r="B4" s="102" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="78" t="s">
         <v>136</v>
-      </c>
-      <c r="C4" s="78" t="s">
-        <v>137</v>
       </c>
       <c r="D4" s="103">
         <v>123456789</v>
@@ -14326,7 +14390,7 @@
   <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14355,7 +14419,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
+      <c r="C2" s="156" t="str">
+        <f>IF(Input!C2="","",Input!C2)</f>
+        <v/>
+      </c>
       <c r="D2" s="156"/>
       <c r="E2" s="156"/>
       <c r="F2" s="156"/>

</xml_diff>